<commit_message>
complete refactoring using headers
</commit_message>
<xml_diff>
--- a/ConsoleApps/LEDReport.xlsx
+++ b/ConsoleApps/LEDReport.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t xml:space="preserve"> SECRET</t>
   </si>
@@ -78,15 +78,9 @@
     <t>Product Data &amp; Configuration Management</t>
   </si>
   <si>
-    <t>Signatures</t>
-  </si>
-  <si>
     <t>Site:</t>
   </si>
   <si>
-    <t>Contacts</t>
-  </si>
-  <si>
     <t>Via Tiburtina Km 12.400</t>
   </si>
   <si>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>Leonardo S.p.a.</t>
+  </si>
+  <si>
+    <t>Point of Contact</t>
   </si>
   <si>
     <t>LEONARDO ELECTRONICS REPORT SAMPLE</t>
@@ -433,6 +430,126 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -442,23 +559,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -474,111 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L210"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1092,26 +1089,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F1" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="F1" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F2" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
+      <c r="F2" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
@@ -1119,15 +1116,15 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="F3" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
+      <c r="F3" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
@@ -1142,20 +1139,20 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
+      <c r="A5" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
@@ -1163,56 +1160,56 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
+      <c r="A7" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
+      <c r="A9" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="67"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
+      <c r="A11" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
@@ -1228,16 +1225,16 @@
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="C14" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
+      <c r="C14" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -1254,16 +1251,16 @@
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="C16" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="69"/>
+      <c r="C16" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1279,68 +1276,68 @@
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="58"/>
+      <c r="C18" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="65"/>
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="58"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="65"/>
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="58"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="65"/>
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="58"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
-      <c r="C22" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="72"/>
+      <c r="C22" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C23" s="22"/>
@@ -1355,16 +1352,16 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="65"/>
+      <c r="C24" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="35"/>
       <c r="K24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1380,16 +1377,16 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="65"/>
+      <c r="C26" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="35"/>
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1425,120 +1422,120 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="73" t="s">
+      <c r="C35" s="50"/>
+      <c r="D35" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="75"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="46"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="49"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B37" s="54">
         <v>10</v>
       </c>
       <c r="C37" s="54"/>
-      <c r="D37" s="59" t="s">
+      <c r="D37" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="61"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B38" s="54"/>
       <c r="C38" s="54"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="61"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B39" s="54"/>
       <c r="C39" s="54"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="61"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B40" s="54"/>
       <c r="C40" s="54"/>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="61"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B41" s="54"/>
       <c r="C41" s="54"/>
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="61"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="54">
         <v>10</v>
       </c>
       <c r="C42" s="54"/>
-      <c r="D42" s="55" t="s">
+      <c r="D42" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G44" s="4"/>
@@ -1578,56 +1575,56 @@
     <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="62" t="s">
+      <c r="A51" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
-      <c r="L51" s="62"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="31"/>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="63"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="63"/>
-      <c r="I52" s="63"/>
-      <c r="J52" s="63"/>
-      <c r="K52" s="63"/>
-      <c r="L52" s="63"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
+      <c r="J52" s="32"/>
+      <c r="K52" s="32"/>
+      <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F53" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="G53" s="49"/>
-      <c r="H53" s="49"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
+      <c r="F53" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="55"/>
+      <c r="H53" s="55"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="55"/>
+      <c r="L53" s="55"/>
     </row>
     <row r="54" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F54" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
+      <c r="F54" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
@@ -1635,23 +1632,21 @@
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
-      <c r="F55" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="50"/>
+      <c r="F55" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="56"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="56"/>
+      <c r="L55" s="56"/>
     </row>
     <row r="57" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="E57" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
@@ -1684,14 +1679,14 @@
       <c r="L60" s="23"/>
     </row>
     <row r="61" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="39"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
+      <c r="F61" s="67"/>
       <c r="G61" s="22"/>
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
@@ -1700,30 +1695,30 @@
       <c r="L61" s="23"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="53"/>
+      <c r="B62" s="69"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="70"/>
+      <c r="G62" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" s="60"/>
+      <c r="I62" s="60"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="61"/>
     </row>
     <row r="63" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
+      <c r="A63" s="74"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
       <c r="G63" s="30"/>
       <c r="H63" s="30"/>
       <c r="I63" s="30"/>
@@ -1746,12 +1741,12 @@
       <c r="L64" s="7"/>
     </row>
     <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="38"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
+      <c r="F65" s="57"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
@@ -1766,12 +1761,12 @@
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="45"/>
-      <c r="J66" s="45"/>
-      <c r="K66" s="45"/>
-      <c r="L66" s="45"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="34"/>
+      <c r="J66" s="34"/>
+      <c r="K66" s="34"/>
+      <c r="L66" s="34"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
@@ -1788,45 +1783,45 @@
       <c r="L67" s="7"/>
     </row>
     <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="E70" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
+      <c r="E70" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E71" s="26"/>
     </row>
     <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="43"/>
-      <c r="L72" s="44"/>
+      <c r="A72" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="76"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="77"/>
+      <c r="G72" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="78"/>
+      <c r="I72" s="78"/>
+      <c r="J72" s="78"/>
+      <c r="K72" s="78"/>
+      <c r="L72" s="79"/>
     </row>
     <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="37" t="s">
+      <c r="A73" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B73" s="38"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="38"/>
-      <c r="F73" s="39"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="57"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="57"/>
+      <c r="F73" s="67"/>
       <c r="G73" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
@@ -1835,50 +1830,50 @@
       <c r="L73" s="23"/>
     </row>
     <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B74" s="32"/>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
-      <c r="E74" s="32"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="L74" s="39"/>
+      <c r="B74" s="72"/>
+      <c r="C74" s="72"/>
+      <c r="D74" s="72"/>
+      <c r="E74" s="72"/>
+      <c r="F74" s="73"/>
+      <c r="G74" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="57"/>
+      <c r="I74" s="57"/>
+      <c r="J74" s="57"/>
+      <c r="K74" s="57"/>
+      <c r="L74" s="67"/>
     </row>
     <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B75" s="32"/>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
-      <c r="L75" s="39"/>
+      <c r="A75" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="72"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="72"/>
+      <c r="E75" s="72"/>
+      <c r="F75" s="73"/>
+      <c r="G75" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="57"/>
+      <c r="I75" s="57"/>
+      <c r="J75" s="57"/>
+      <c r="K75" s="57"/>
+      <c r="L75" s="67"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A76" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="B76" s="35"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
-      <c r="F76" s="36"/>
+      <c r="A76" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" s="69"/>
+      <c r="C76" s="69"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="70"/>
       <c r="G76" s="17"/>
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
@@ -1901,26 +1896,26 @@
       <c r="L104" s="17"/>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F105" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="G105" s="49"/>
-      <c r="H105" s="49"/>
-      <c r="I105" s="49"/>
-      <c r="J105" s="49"/>
-      <c r="K105" s="49"/>
-      <c r="L105" s="49"/>
+      <c r="F105" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="55"/>
+      <c r="J105" s="55"/>
+      <c r="K105" s="55"/>
+      <c r="L105" s="55"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F106" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G106" s="49"/>
-      <c r="H106" s="49"/>
-      <c r="I106" s="49"/>
-      <c r="J106" s="49"/>
-      <c r="K106" s="49"/>
-      <c r="L106" s="49"/>
+      <c r="F106" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G106" s="55"/>
+      <c r="H106" s="55"/>
+      <c r="I106" s="55"/>
+      <c r="J106" s="55"/>
+      <c r="K106" s="55"/>
+      <c r="L106" s="55"/>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="17"/>
@@ -1928,15 +1923,15 @@
       <c r="C107" s="17"/>
       <c r="D107" s="17"/>
       <c r="E107" s="17"/>
-      <c r="F107" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G107" s="50"/>
-      <c r="H107" s="50"/>
-      <c r="I107" s="50"/>
-      <c r="J107" s="50"/>
-      <c r="K107" s="50"/>
-      <c r="L107" s="50"/>
+      <c r="F107" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G107" s="56"/>
+      <c r="H107" s="56"/>
+      <c r="I107" s="56"/>
+      <c r="J107" s="56"/>
+      <c r="K107" s="56"/>
+      <c r="L107" s="56"/>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
@@ -1995,26 +1990,26 @@
       <c r="L157" s="17"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F158" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="G158" s="49"/>
-      <c r="H158" s="49"/>
-      <c r="I158" s="49"/>
-      <c r="J158" s="49"/>
-      <c r="K158" s="49"/>
-      <c r="L158" s="49"/>
+      <c r="F158" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G158" s="55"/>
+      <c r="H158" s="55"/>
+      <c r="I158" s="55"/>
+      <c r="J158" s="55"/>
+      <c r="K158" s="55"/>
+      <c r="L158" s="55"/>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F159" s="49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G159" s="49"/>
-      <c r="H159" s="49"/>
-      <c r="I159" s="49"/>
-      <c r="J159" s="49"/>
-      <c r="K159" s="49"/>
-      <c r="L159" s="49"/>
+      <c r="F159" s="55" t="s">
+        <v>20</v>
+      </c>
+      <c r="G159" s="55"/>
+      <c r="H159" s="55"/>
+      <c r="I159" s="55"/>
+      <c r="J159" s="55"/>
+      <c r="K159" s="55"/>
+      <c r="L159" s="55"/>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="17"/>
@@ -2022,15 +2017,15 @@
       <c r="C160" s="17"/>
       <c r="D160" s="17"/>
       <c r="E160" s="17"/>
-      <c r="F160" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G160" s="50"/>
-      <c r="H160" s="50"/>
-      <c r="I160" s="50"/>
-      <c r="J160" s="50"/>
-      <c r="K160" s="50"/>
-      <c r="L160" s="50"/>
+      <c r="F160" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G160" s="56"/>
+      <c r="H160" s="56"/>
+      <c r="I160" s="56"/>
+      <c r="J160" s="56"/>
+      <c r="K160" s="56"/>
+      <c r="L160" s="56"/>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="7"/>
@@ -2118,18 +2113,38 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="G75:L75"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="G72:L72"/>
+    <mergeCell ref="G74:L74"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="G66:L66"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="E57:H57"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="E70:H70"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="F55:L55"/>
+    <mergeCell ref="F54:L54"/>
+    <mergeCell ref="F53:L53"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="C18:J21"/>
+    <mergeCell ref="A61:F61"/>
     <mergeCell ref="F158:L158"/>
     <mergeCell ref="F159:L159"/>
     <mergeCell ref="F160:L160"/>
     <mergeCell ref="F105:L105"/>
     <mergeCell ref="F106:L106"/>
     <mergeCell ref="F107:L107"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="C18:J21"/>
-    <mergeCell ref="A61:F61"/>
     <mergeCell ref="D39:K39"/>
     <mergeCell ref="D40:K40"/>
     <mergeCell ref="B37:C37"/>
@@ -2138,45 +2153,28 @@
     <mergeCell ref="A51:L52"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="D35:K36"/>
-    <mergeCell ref="B35:C36"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="F55:L55"/>
-    <mergeCell ref="F54:L54"/>
-    <mergeCell ref="F53:L53"/>
     <mergeCell ref="C14:J14"/>
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="C16:J16"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="D35:K36"/>
+    <mergeCell ref="B35:C36"/>
     <mergeCell ref="D41:K41"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D37:K37"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="G66:L66"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="E57:H57"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="E70:H70"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="G75:L75"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="G72:L72"/>
-    <mergeCell ref="G74:L74"/>
-    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="D38:K38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="200" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Arial,Bold"&amp;KFF0000UNCLASSIFIED</oddHeader>
-    <oddFooter>&amp;LTemplate: CFM001-T-IT-L en rev.  04.00&amp;C&amp;"Arial,Bold"&amp;KFF0000UNCLASSIFIED&amp;Rpage &amp;P of &amp;N</oddFooter>
+    <oddFooter xml:space="preserve">&amp;L&amp;8Template: CFM001-T-IT-I en rev. 04.02
+&amp;C&amp;"Arial,Bold"&amp;8© Copyright Leonardo S.p.a. All Rights Reserved&amp;11&amp;KFF0000
+ UNCLASSIFIED&amp;R&amp;9page &amp;P of &amp;N
+</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>